<commit_message>
New files for corrected test cases (233,234,235) and inserted missing 39,374 test cases
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#CGMXX/CGM_XDENT_SOFTWARE_SRL/CGMXFSE/1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#CGMXX/CGM_XDENT_SOFTWARE_SRL/CGMXFSE/1/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/michele_bukovitz_cgm_com/Documents/Documentazione/FSE/ACCREDITAMENTO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="280" documentId="8_{45AC9EDC-DA0E-934D-A942-652691440C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25774FB3-B1E4-3046-81D8-524C452F01B1}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="8_{45AC9EDC-DA0E-934D-A942-652691440C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7F7203D-4BDA-344D-9025-7FA6A1007CE7}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="500" windowWidth="34960" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1600" yWindow="500" windowWidth="34960" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="394">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -451,9 +451,6 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
-    <t>eae46e77434195d0</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_RAD_TIMEOUT</t>
   </si>
   <si>
@@ -699,15 +696,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2024-04-10T10:01:52Z</t>
-  </si>
-  <si>
-    <t>f065ba2899c96918</t>
-  </si>
-  <si>
-    <t>0.1.2.3.4.9ae2bdd7beedc2e766c6b76585530e16925115707dc7a06ab5ee4aa2776b2c7b.4d8555878a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT9_KO</t>
@@ -1441,9 +1429,6 @@
     <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.79fdb96c30^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2024-04-19T09:58:56</t>
-  </si>
-  <si>
     <t>d37d939bbcb71afb</t>
   </si>
   <si>
@@ -1544,21 +1529,6 @@
   </si>
   <si>
     <t>8437a00129d494e9</t>
-  </si>
-  <si>
-    <t>2024-04-19T11:14:05Z</t>
-  </si>
-  <si>
-    <t>89b2c356c9e3fb0a</t>
-  </si>
-  <si>
-    <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.025be7d292^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-04-19T11:16:53Z</t>
-  </si>
-  <si>
-    <t>2024-04-19T11:18:27Z</t>
   </si>
   <si>
     <t>2024-04-19T11:32:16Z</t>
@@ -1636,6 +1606,48 @@
   </si>
   <si>
     <t>2024-04-18T18:37:33Z</t>
+  </si>
+  <si>
+    <t>8c0960676c99b8b0</t>
+  </si>
+  <si>
+    <t>2024-04-19T09:58:56Z</t>
+  </si>
+  <si>
+    <t>2024-04-18T17:05:13Z</t>
+  </si>
+  <si>
+    <t>f199b2399af55115</t>
+  </si>
+  <si>
+    <t>0.1.2.3.4.043066daf2109523a7490d4bfad4766da5719950a2b5f96d192fc0537e84f32a.53c05b9459^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-03T10:01:51Z</t>
+  </si>
+  <si>
+    <t>228b19aaea321718</t>
+  </si>
+  <si>
+    <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.2494d5c541^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-03T10:05:47Z</t>
+  </si>
+  <si>
+    <t>43931460a10213c1</t>
+  </si>
+  <si>
+    <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.2093eb6648^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-03T10:07:35Z</t>
+  </si>
+  <si>
+    <t>ffa2031ef7c1a65e</t>
+  </si>
+  <si>
+    <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.8cba2b19d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2169,6 +2181,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4552,13 +4568,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T700"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D79" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="79" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G77" sqref="G77"/>
+      <selection pane="bottomRight" activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4820,22 +4837,22 @@
         <v>48</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="F10" s="23">
         <v>45405</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>52</v>
@@ -4850,10 +4867,10 @@
       <c r="R10" s="26"/>
       <c r="S10" s="27"/>
       <c r="T10" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>12</v>
       </c>
@@ -4864,10 +4881,10 @@
         <v>48</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="F11" s="23">
         <v>45406</v>
@@ -4876,10 +4893,10 @@
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
       <c r="J11" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
@@ -4890,10 +4907,10 @@
       <c r="R11" s="26"/>
       <c r="S11" s="27"/>
       <c r="T11" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>13</v>
       </c>
@@ -4904,10 +4921,10 @@
         <v>48</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="F12" s="23">
         <v>45407</v>
@@ -4916,10 +4933,10 @@
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
       <c r="J12" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>
@@ -4930,10 +4947,10 @@
       <c r="R12" s="26"/>
       <c r="S12" s="27"/>
       <c r="T12" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>14</v>
       </c>
@@ -4944,10 +4961,10 @@
         <v>48</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F13" s="23">
         <v>45408</v>
@@ -4956,10 +4973,10 @@
       <c r="H13" s="24"/>
       <c r="I13" s="24"/>
       <c r="J13" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K13" s="25" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -4970,7 +4987,7 @@
       <c r="R13" s="26"/>
       <c r="S13" s="27"/>
       <c r="T13" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
@@ -4993,10 +5010,10 @@
         <v>45401</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I14" s="24" t="s">
         <v>51</v>
@@ -5015,7 +5032,7 @@
         <v>53</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P14" s="25" t="s">
         <v>54</v>
@@ -5047,10 +5064,10 @@
         <v>45400</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>51</v>
@@ -5069,7 +5086,7 @@
         <v>53</v>
       </c>
       <c r="O15" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P15" s="25" t="s">
         <v>54</v>
@@ -5101,10 +5118,10 @@
         <v>45401</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>51</v>
@@ -5123,7 +5140,7 @@
         <v>53</v>
       </c>
       <c r="O16" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P16" s="25" t="s">
         <v>54</v>
@@ -5155,10 +5172,10 @@
         <v>45400</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>62</v>
+        <v>380</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>51</v>
@@ -5177,7 +5194,7 @@
         <v>53</v>
       </c>
       <c r="O17" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P17" s="25" t="s">
         <v>54</v>
@@ -5189,7 +5206,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="65" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>47</v>
       </c>
@@ -5200,10 +5217,10 @@
         <v>48</v>
       </c>
       <c r="D18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="22" t="s">
         <v>63</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>64</v>
       </c>
       <c r="F18" s="23">
         <v>45401</v>
@@ -5226,7 +5243,7 @@
         <v>52</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="26" t="s">
@@ -5248,16 +5265,16 @@
         <v>57</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F19" s="23">
         <v>45391</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
@@ -5278,7 +5295,7 @@
         <v>52</v>
       </c>
       <c r="P19" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26" t="s">
@@ -5300,22 +5317,22 @@
         <v>48</v>
       </c>
       <c r="D20" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="22" t="s">
         <v>68</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>69</v>
       </c>
       <c r="F20" s="23">
         <v>45401</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>52</v>
@@ -5331,7 +5348,7 @@
         <v>53</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P20" s="25" t="s">
         <v>54</v>
@@ -5354,22 +5371,22 @@
         <v>48</v>
       </c>
       <c r="D21" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="22" t="s">
         <v>70</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>71</v>
       </c>
       <c r="F21" s="23">
         <v>45401</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>327</v>
+        <v>381</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>52</v>
@@ -5385,7 +5402,7 @@
         <v>53</v>
       </c>
       <c r="O21" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P21" s="25" t="s">
         <v>54</v>
@@ -5408,22 +5425,22 @@
         <v>48</v>
       </c>
       <c r="D22" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="22" t="s">
         <v>72</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>73</v>
       </c>
       <c r="F22" s="23">
         <v>45401</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>52</v>
@@ -5439,7 +5456,7 @@
         <v>53</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P22" s="25" t="s">
         <v>54</v>
@@ -5462,22 +5479,22 @@
         <v>48</v>
       </c>
       <c r="D23" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="22" t="s">
         <v>74</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>75</v>
       </c>
       <c r="F23" s="23">
         <v>45401</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>52</v>
@@ -5493,7 +5510,7 @@
         <v>53</v>
       </c>
       <c r="O23" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P23" s="25" t="s">
         <v>54</v>
@@ -5516,22 +5533,22 @@
         <v>48</v>
       </c>
       <c r="D24" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="22" t="s">
         <v>76</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>77</v>
       </c>
       <c r="F24" s="23">
         <v>45401</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>52</v>
@@ -5547,7 +5564,7 @@
         <v>53</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P24" s="25" t="s">
         <v>54</v>
@@ -5570,22 +5587,22 @@
         <v>48</v>
       </c>
       <c r="D25" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="22" t="s">
         <v>78</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>79</v>
       </c>
       <c r="F25" s="23">
         <v>45401</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>52</v>
@@ -5601,7 +5618,7 @@
         <v>53</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P25" s="25" t="s">
         <v>54</v>
@@ -5613,7 +5630,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>81</v>
       </c>
@@ -5624,20 +5641,20 @@
         <v>48</v>
       </c>
       <c r="D26" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="22" t="s">
         <v>80</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>81</v>
       </c>
       <c r="F26" s="23"/>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
       <c r="I26" s="24"/>
       <c r="J26" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="K26" s="25" t="s">
         <v>82</v>
-      </c>
-      <c r="K26" s="25" t="s">
-        <v>83</v>
       </c>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
@@ -5662,22 +5679,22 @@
         <v>48</v>
       </c>
       <c r="D27" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="22" t="s">
         <v>84</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>85</v>
       </c>
       <c r="F27" s="23">
         <v>45401</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>52</v>
@@ -5693,7 +5710,7 @@
         <v>53</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P27" s="25" t="s">
         <v>54</v>
@@ -5705,7 +5722,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>83</v>
       </c>
@@ -5716,20 +5733,20 @@
         <v>48</v>
       </c>
       <c r="D28" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="22" t="s">
         <v>86</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>87</v>
       </c>
       <c r="F28" s="23"/>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
       <c r="I28" s="24"/>
       <c r="J28" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L28" s="25"/>
       <c r="M28" s="25"/>
@@ -5754,22 +5771,22 @@
         <v>48</v>
       </c>
       <c r="D29" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="F29" s="23">
         <v>45401</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="J29" s="25" t="s">
         <v>52</v>
@@ -5785,7 +5802,7 @@
         <v>53</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P29" s="25" t="s">
         <v>54</v>
@@ -5808,22 +5825,22 @@
         <v>48</v>
       </c>
       <c r="D30" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="22" t="s">
         <v>91</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>92</v>
       </c>
       <c r="F30" s="23">
         <v>45401</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="H30" s="24" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="J30" s="25" t="s">
         <v>52</v>
@@ -5839,7 +5856,7 @@
         <v>53</v>
       </c>
       <c r="O30" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P30" s="25" t="s">
         <v>54</v>
@@ -5851,7 +5868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <v>86</v>
       </c>
@@ -5862,20 +5879,20 @@
         <v>48</v>
       </c>
       <c r="D31" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>93</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>94</v>
       </c>
       <c r="F31" s="23"/>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
       <c r="I31" s="24"/>
       <c r="J31" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
@@ -5889,7 +5906,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
         <v>87</v>
       </c>
@@ -5900,20 +5917,20 @@
         <v>48</v>
       </c>
       <c r="D32" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="22" t="s">
         <v>96</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>97</v>
       </c>
       <c r="F32" s="23"/>
       <c r="G32" s="24"/>
       <c r="H32" s="24"/>
       <c r="I32" s="24"/>
       <c r="J32" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K32" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L32" s="25"/>
       <c r="M32" s="25"/>
@@ -5927,7 +5944,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <v>88</v>
       </c>
@@ -5938,20 +5955,20 @@
         <v>48</v>
       </c>
       <c r="D33" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="22" t="s">
         <v>98</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>99</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
       <c r="I33" s="24"/>
       <c r="J33" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K33" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
@@ -5965,7 +5982,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
         <v>89</v>
       </c>
@@ -5976,20 +5993,20 @@
         <v>48</v>
       </c>
       <c r="D34" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>100</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>101</v>
       </c>
       <c r="F34" s="23"/>
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
       <c r="I34" s="24"/>
       <c r="J34" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K34" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L34" s="25"/>
       <c r="M34" s="25"/>
@@ -6003,7 +6020,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
         <v>90</v>
       </c>
@@ -6014,20 +6031,20 @@
         <v>48</v>
       </c>
       <c r="D35" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>102</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>103</v>
       </c>
       <c r="F35" s="23"/>
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
       <c r="I35" s="24"/>
       <c r="J35" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K35" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
@@ -6041,7 +6058,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <v>91</v>
       </c>
@@ -6052,20 +6069,20 @@
         <v>48</v>
       </c>
       <c r="D36" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>105</v>
       </c>
       <c r="F36" s="23"/>
       <c r="G36" s="24"/>
       <c r="H36" s="24"/>
       <c r="I36" s="24"/>
       <c r="J36" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K36" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L36" s="25"/>
       <c r="M36" s="25"/>
@@ -6079,7 +6096,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
         <v>92</v>
       </c>
@@ -6090,20 +6107,20 @@
         <v>48</v>
       </c>
       <c r="D37" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="22" t="s">
         <v>106</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>107</v>
       </c>
       <c r="F37" s="23"/>
       <c r="G37" s="24"/>
       <c r="H37" s="24"/>
       <c r="I37" s="24"/>
       <c r="J37" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L37" s="25"/>
       <c r="M37" s="25"/>
@@ -6117,7 +6134,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
         <v>93</v>
       </c>
@@ -6128,20 +6145,20 @@
         <v>48</v>
       </c>
       <c r="D38" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="22" t="s">
         <v>108</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>109</v>
       </c>
       <c r="F38" s="23"/>
       <c r="G38" s="24"/>
       <c r="H38" s="24"/>
       <c r="I38" s="24"/>
       <c r="J38" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L38" s="25"/>
       <c r="M38" s="25"/>
@@ -6155,7 +6172,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="161" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
         <v>147</v>
       </c>
@@ -6166,20 +6183,20 @@
         <v>57</v>
       </c>
       <c r="D39" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="22" t="s">
         <v>110</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>111</v>
       </c>
       <c r="F39" s="23"/>
       <c r="G39" s="24"/>
       <c r="H39" s="24"/>
       <c r="I39" s="24"/>
       <c r="J39" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K39" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L39" s="25"/>
       <c r="M39" s="25"/>
@@ -6190,10 +6207,10 @@
       <c r="R39" s="26"/>
       <c r="S39" s="27"/>
       <c r="T39" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="161" thickBot="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
         <v>148</v>
       </c>
@@ -6204,20 +6221,20 @@
         <v>57</v>
       </c>
       <c r="D40" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" s="22" t="s">
         <v>113</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>114</v>
       </c>
       <c r="F40" s="23"/>
       <c r="G40" s="24"/>
       <c r="H40" s="24"/>
       <c r="I40" s="24"/>
       <c r="J40" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K40" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L40" s="25"/>
       <c r="M40" s="25"/>
@@ -6228,10 +6245,10 @@
       <c r="R40" s="26"/>
       <c r="S40" s="27"/>
       <c r="T40" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" ht="161" thickBot="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
         <v>149</v>
       </c>
@@ -6242,20 +6259,20 @@
         <v>57</v>
       </c>
       <c r="D41" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="22" t="s">
         <v>115</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>116</v>
       </c>
       <c r="F41" s="23"/>
       <c r="G41" s="24"/>
       <c r="H41" s="24"/>
       <c r="I41" s="24"/>
       <c r="J41" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K41" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L41" s="25"/>
       <c r="M41" s="25"/>
@@ -6266,10 +6283,10 @@
       <c r="R41" s="26"/>
       <c r="S41" s="27"/>
       <c r="T41" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" ht="161" thickBot="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <v>150</v>
       </c>
@@ -6280,20 +6297,20 @@
         <v>57</v>
       </c>
       <c r="D42" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" s="22" t="s">
         <v>117</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>118</v>
       </c>
       <c r="F42" s="23"/>
       <c r="G42" s="24"/>
       <c r="H42" s="24"/>
       <c r="I42" s="24"/>
       <c r="J42" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K42" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L42" s="25"/>
       <c r="M42" s="25"/>
@@ -6304,7 +6321,7 @@
       <c r="R42" s="26"/>
       <c r="S42" s="27"/>
       <c r="T42" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
@@ -6318,22 +6335,22 @@
         <v>57</v>
       </c>
       <c r="D43" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="22" t="s">
         <v>119</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>120</v>
       </c>
       <c r="F43" s="23">
         <v>45400</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>52</v>
@@ -6349,7 +6366,7 @@
         <v>53</v>
       </c>
       <c r="O43" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P43" s="25" t="s">
         <v>54</v>
@@ -6372,22 +6389,22 @@
         <v>57</v>
       </c>
       <c r="D44" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E44" s="22" t="s">
         <v>121</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>122</v>
       </c>
       <c r="F44" s="23">
         <v>45400</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>128</v>
+        <v>382</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>129</v>
+        <v>383</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>130</v>
+        <v>384</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>52</v>
@@ -6403,7 +6420,7 @@
         <v>53</v>
       </c>
       <c r="O44" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P44" s="25" t="s">
         <v>54</v>
@@ -6415,7 +6432,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
         <v>153</v>
       </c>
@@ -6426,20 +6443,20 @@
         <v>57</v>
       </c>
       <c r="D45" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" s="22" t="s">
         <v>123</v>
-      </c>
-      <c r="E45" s="22" t="s">
-        <v>124</v>
       </c>
       <c r="F45" s="23"/>
       <c r="G45" s="24"/>
       <c r="H45" s="24"/>
       <c r="I45" s="24"/>
       <c r="J45" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K45" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L45" s="25"/>
       <c r="M45" s="25"/>
@@ -6464,22 +6481,22 @@
         <v>57</v>
       </c>
       <c r="D46" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" s="22" t="s">
         <v>126</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>127</v>
       </c>
       <c r="F46" s="23">
         <v>45400</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>52</v>
@@ -6495,7 +6512,7 @@
         <v>53</v>
       </c>
       <c r="O46" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P46" s="25" t="s">
         <v>54</v>
@@ -6518,22 +6535,22 @@
         <v>57</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F47" s="23">
         <v>45400</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>52</v>
@@ -6549,7 +6566,7 @@
         <v>53</v>
       </c>
       <c r="O47" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P47" s="25" t="s">
         <v>54</v>
@@ -6572,22 +6589,22 @@
         <v>57</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F48" s="23">
         <v>45400</v>
       </c>
       <c r="G48" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="H48" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="I48" s="24" t="s">
         <v>285</v>
-      </c>
-      <c r="H48" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="I48" s="24" t="s">
-        <v>289</v>
       </c>
       <c r="J48" s="25" t="s">
         <v>52</v>
@@ -6603,7 +6620,7 @@
         <v>53</v>
       </c>
       <c r="O48" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P48" s="25" t="s">
         <v>54</v>
@@ -6615,7 +6632,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20">
         <v>157</v>
       </c>
@@ -6626,20 +6643,20 @@
         <v>57</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F49" s="23"/>
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
       <c r="I49" s="24"/>
       <c r="J49" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K49" s="25" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L49" s="25"/>
       <c r="M49" s="25"/>
@@ -6664,22 +6681,22 @@
         <v>57</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F50" s="23">
         <v>45400</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="H50" s="24" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="J50" s="25" t="s">
         <v>52</v>
@@ -6695,7 +6712,7 @@
         <v>53</v>
       </c>
       <c r="O50" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P50" s="25" t="s">
         <v>54</v>
@@ -6718,22 +6735,22 @@
         <v>57</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F51" s="23">
         <v>45400</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J51" s="25" t="s">
         <v>52</v>
@@ -6749,7 +6766,7 @@
         <v>53</v>
       </c>
       <c r="O51" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P51" s="25" t="s">
         <v>54</v>
@@ -6772,22 +6789,22 @@
         <v>57</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F52" s="23">
         <v>45400</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="H52" s="24" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="I52" s="24" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="J52" s="25" t="s">
         <v>52</v>
@@ -6803,7 +6820,7 @@
         <v>53</v>
       </c>
       <c r="O52" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P52" s="25" t="s">
         <v>54</v>
@@ -6826,22 +6843,22 @@
         <v>57</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F53" s="23">
         <v>45400</v>
       </c>
       <c r="G53" s="24" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H53" s="23" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="I53" s="24" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="J53" s="25" t="s">
         <v>52</v>
@@ -6857,7 +6874,7 @@
         <v>53</v>
       </c>
       <c r="O53" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P53" s="25" t="s">
         <v>54</v>
@@ -6869,7 +6886,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
         <v>162</v>
       </c>
@@ -6880,20 +6897,20 @@
         <v>57</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F54" s="23"/>
       <c r="G54" s="24"/>
       <c r="H54" s="24"/>
       <c r="I54" s="24"/>
       <c r="J54" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K54" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L54" s="25"/>
       <c r="M54" s="25"/>
@@ -6907,7 +6924,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
         <v>163</v>
       </c>
@@ -6918,20 +6935,20 @@
         <v>57</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="24"/>
       <c r="H55" s="24"/>
       <c r="I55" s="24"/>
       <c r="J55" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K55" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
@@ -6945,7 +6962,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
         <v>164</v>
       </c>
@@ -6956,20 +6973,20 @@
         <v>57</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F56" s="23"/>
       <c r="G56" s="24"/>
       <c r="H56" s="24"/>
       <c r="I56" s="24"/>
       <c r="J56" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K56" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L56" s="25"/>
       <c r="M56" s="25"/>
@@ -6983,7 +7000,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
         <v>165</v>
       </c>
@@ -6994,20 +7011,20 @@
         <v>57</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F57" s="23"/>
       <c r="G57" s="24"/>
       <c r="H57" s="24"/>
       <c r="I57" s="24"/>
       <c r="J57" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K57" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L57" s="25"/>
       <c r="M57" s="25"/>
@@ -7021,7 +7038,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
         <v>166</v>
       </c>
@@ -7032,20 +7049,20 @@
         <v>57</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F58" s="23"/>
       <c r="G58" s="24"/>
       <c r="H58" s="24"/>
       <c r="I58" s="24"/>
       <c r="J58" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K58" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L58" s="25"/>
       <c r="M58" s="25"/>
@@ -7059,7 +7076,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20">
         <v>167</v>
       </c>
@@ -7070,20 +7087,20 @@
         <v>57</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F59" s="23"/>
       <c r="G59" s="24"/>
       <c r="H59" s="24"/>
       <c r="I59" s="24"/>
       <c r="J59" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K59" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L59" s="25"/>
       <c r="M59" s="25"/>
@@ -7097,7 +7114,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20">
         <v>168</v>
       </c>
@@ -7108,20 +7125,20 @@
         <v>57</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F60" s="23"/>
       <c r="G60" s="24"/>
       <c r="H60" s="24"/>
       <c r="I60" s="24"/>
       <c r="J60" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K60" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L60" s="25"/>
       <c r="M60" s="25"/>
@@ -7135,7 +7152,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
         <v>169</v>
       </c>
@@ -7146,20 +7163,20 @@
         <v>57</v>
       </c>
       <c r="D61" s="21" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F61" s="23"/>
       <c r="G61" s="24"/>
       <c r="H61" s="24"/>
       <c r="I61" s="24"/>
       <c r="J61" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K61" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L61" s="25"/>
       <c r="M61" s="25"/>
@@ -7178,28 +7195,28 @@
         <v>224</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C62" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F62" s="23">
         <v>45401</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="H62" s="24" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="J62" s="25" t="s">
         <v>52</v>
@@ -7214,34 +7231,34 @@
       <c r="R62" s="26"/>
       <c r="S62" s="27"/>
       <c r="T62" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" ht="177" thickBot="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" ht="177" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
         <v>229</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C63" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D63" s="21" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F63" s="23"/>
       <c r="G63" s="24"/>
       <c r="H63" s="24"/>
       <c r="I63" s="24"/>
       <c r="J63" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K63" s="25" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L63" s="25"/>
       <c r="M63" s="25"/>
@@ -7260,28 +7277,28 @@
         <v>230</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C64" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F64" s="23">
         <v>45401</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H64" s="24" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I64" s="24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J64" s="25" t="s">
         <v>52</v>
@@ -7294,13 +7311,13 @@
         <v>52</v>
       </c>
       <c r="N64" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O64" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P64" s="25" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="Q64" s="25"/>
       <c r="R64" s="26"/>
@@ -7314,28 +7331,28 @@
         <v>231</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C65" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F65" s="23">
         <v>45401</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="H65" s="24" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J65" s="25" t="s">
         <v>52</v>
@@ -7348,13 +7365,13 @@
         <v>52</v>
       </c>
       <c r="N65" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O65" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P65" s="25" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="Q65" s="25"/>
       <c r="R65" s="26"/>
@@ -7368,28 +7385,28 @@
         <v>232</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C66" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F66" s="23">
         <v>45401</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="H66" s="24" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I66" s="24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J66" s="25" t="s">
         <v>52</v>
@@ -7402,13 +7419,13 @@
         <v>52</v>
       </c>
       <c r="N66" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O66" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P66" s="25" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="Q66" s="25"/>
       <c r="R66" s="26"/>
@@ -7422,47 +7439,47 @@
         <v>233</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C67" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F67" s="23">
-        <v>45401</v>
+        <v>45415</v>
       </c>
       <c r="G67" s="24" t="s">
-        <v>362</v>
+        <v>385</v>
       </c>
       <c r="H67" s="24" t="s">
-        <v>363</v>
+        <v>386</v>
       </c>
       <c r="I67" s="24" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
       <c r="J67" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K67" s="25"/>
       <c r="L67" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M67" s="25" t="s">
         <v>52</v>
       </c>
       <c r="N67" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="O67" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P67" s="25" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="26"/>
@@ -7476,47 +7493,47 @@
         <v>234</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C68" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F68" s="23">
-        <v>45401</v>
+        <v>45415</v>
       </c>
       <c r="G68" s="24" t="s">
-        <v>365</v>
+        <v>388</v>
       </c>
       <c r="H68" s="24" t="s">
-        <v>363</v>
+        <v>389</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>364</v>
+        <v>390</v>
       </c>
       <c r="J68" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K68" s="25"/>
       <c r="L68" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M68" s="25" t="s">
         <v>52</v>
       </c>
       <c r="N68" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="O68" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P68" s="25" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="Q68" s="25"/>
       <c r="R68" s="26"/>
@@ -7530,47 +7547,47 @@
         <v>235</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C69" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F69" s="23">
-        <v>45401</v>
+        <v>45415</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>366</v>
+        <v>391</v>
       </c>
       <c r="H69" s="24" t="s">
-        <v>363</v>
+        <v>392</v>
       </c>
       <c r="I69" s="24" t="s">
-        <v>364</v>
+        <v>393</v>
       </c>
       <c r="J69" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K69" s="25"/>
       <c r="L69" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M69" s="25" t="s">
         <v>52</v>
       </c>
       <c r="N69" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="O69" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P69" s="25" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="Q69" s="25"/>
       <c r="R69" s="26"/>
@@ -7584,28 +7601,28 @@
         <v>288</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C70" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F70" s="23">
         <v>45400</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="H70" s="24" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="J70" s="25" t="s">
         <v>52</v>
@@ -7620,34 +7637,34 @@
       <c r="R70" s="26"/>
       <c r="S70" s="27"/>
       <c r="T70" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" ht="177" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="177" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="20">
         <v>293</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C71" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F71" s="23"/>
       <c r="G71" s="24"/>
       <c r="H71" s="24"/>
       <c r="I71" s="24"/>
       <c r="J71" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K71" s="25" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L71" s="25"/>
       <c r="M71" s="25"/>
@@ -7666,28 +7683,28 @@
         <v>294</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C72" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F72" s="23">
         <v>45400</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J72" s="25" t="s">
         <v>52</v>
@@ -7700,13 +7717,13 @@
         <v>52</v>
       </c>
       <c r="N72" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O72" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P72" s="25" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="Q72" s="25"/>
       <c r="R72" s="26"/>
@@ -7720,28 +7737,28 @@
         <v>295</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C73" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E73" s="22" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F73" s="23">
         <v>45400</v>
       </c>
       <c r="G73" s="24" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="H73" s="24" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="I73" s="24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J73" s="25" t="s">
         <v>52</v>
@@ -7754,13 +7771,13 @@
         <v>52</v>
       </c>
       <c r="N73" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O73" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P73" s="25" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="Q73" s="25"/>
       <c r="R73" s="26"/>
@@ -7774,28 +7791,28 @@
         <v>296</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C74" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D74" s="21" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F74" s="23">
         <v>45400</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="I74" s="24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J74" s="25" t="s">
         <v>52</v>
@@ -7808,13 +7825,13 @@
         <v>52</v>
       </c>
       <c r="N74" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O74" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P74" s="25" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="Q74" s="25"/>
       <c r="R74" s="26"/>
@@ -7828,47 +7845,47 @@
         <v>297</v>
       </c>
       <c r="B75" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C75" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F75" s="23">
         <v>45400</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="H75" s="24" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I75" s="24" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="J75" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K75" s="25"/>
       <c r="L75" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M75" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N75" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="O75" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P75" s="25" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q75" s="25"/>
       <c r="R75" s="26"/>
@@ -7882,47 +7899,47 @@
         <v>298</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C76" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F76" s="23">
         <v>45400</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="H76" s="24" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="I76" s="24" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="J76" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K76" s="25"/>
       <c r="L76" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M76" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N76" s="25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O76" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P76" s="25" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q76" s="25"/>
       <c r="R76" s="26"/>
@@ -7936,47 +7953,47 @@
         <v>299</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C77" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F77" s="23">
         <v>45400</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="H77" s="24" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="I77" s="24" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="J77" s="25" t="s">
         <v>52</v>
       </c>
       <c r="K77" s="25"/>
       <c r="L77" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M77" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N77" s="25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O77" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P77" s="25" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q77" s="25"/>
       <c r="R77" s="26"/>
@@ -7990,28 +8007,28 @@
         <v>328</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C78" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F78" s="23">
         <v>45401</v>
       </c>
       <c r="G78" s="24" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="H78" s="24" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="I78" s="24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J78" s="25" t="s">
         <v>52</v>
@@ -8024,7 +8041,7 @@
         <v>52</v>
       </c>
       <c r="N78" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O78" s="25"/>
       <c r="P78" s="25" t="s">
@@ -8042,28 +8059,28 @@
         <v>329</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C79" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E79" s="22" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F79" s="23">
         <v>45401</v>
       </c>
       <c r="G79" s="24" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="H79" s="24" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="I79" s="24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J79" s="25" t="s">
         <v>52</v>
@@ -8076,7 +8093,7 @@
         <v>52</v>
       </c>
       <c r="N79" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O79" s="25"/>
       <c r="P79" s="25" t="s">
@@ -8089,31 +8106,31 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="242.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="242.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
         <v>344</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C80" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D80" s="21" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E80" s="22" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F80" s="23"/>
       <c r="G80" s="24"/>
       <c r="H80" s="24"/>
       <c r="I80" s="24"/>
       <c r="J80" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="K80" s="25" t="s">
         <v>82</v>
-      </c>
-      <c r="K80" s="25" t="s">
-        <v>83</v>
       </c>
       <c r="L80" s="25"/>
       <c r="M80" s="25"/>
@@ -8132,28 +8149,28 @@
         <v>345</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C81" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D81" s="21" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F81" s="23">
         <v>45400</v>
       </c>
       <c r="G81" s="24" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H81" s="24" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="I81" s="24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J81" s="25" t="s">
         <v>52</v>
@@ -8166,13 +8183,13 @@
         <v>52</v>
       </c>
       <c r="N81" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O81" s="25" t="s">
         <v>52</v>
       </c>
       <c r="P81" s="25" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="Q81" s="25"/>
       <c r="R81" s="26"/>
@@ -8192,22 +8209,22 @@
         <v>48</v>
       </c>
       <c r="D82" s="21" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E82" s="22" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F82" s="23">
         <v>45401</v>
       </c>
       <c r="G82" s="24" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="H82" s="24" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="J82" s="25" t="s">
         <v>52</v>
@@ -8222,7 +8239,7 @@
       <c r="R82" s="26"/>
       <c r="S82" s="27"/>
       <c r="T82" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="1:20" ht="160" x14ac:dyDescent="0.2">
@@ -8236,22 +8253,22 @@
         <v>57</v>
       </c>
       <c r="D83" s="21" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F83" s="23">
         <v>45400</v>
       </c>
       <c r="G83" s="24" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="H83" s="24" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="I83" s="24" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="J83" s="25" t="s">
         <v>52</v>
@@ -8266,7 +8283,7 @@
       <c r="R83" s="26"/>
       <c r="S83" s="27"/>
       <c r="T83" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12921,7 +12938,13 @@
       <c r="T700" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T83" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A9:T83" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="SI"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -12981,38 +13004,38 @@
         <v>28</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>221</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>225</v>
-      </c>
       <c r="D3" s="30" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13020,55 +13043,55 @@
         <v>48</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -13076,69 +13099,69 @@
         <v>57</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C11" s="30">
         <v>192</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C12" s="30">
         <v>208</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13146,55 +13169,55 @@
         <v>48</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C13" s="30">
         <v>224</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C14" s="30">
         <v>240</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C15" s="30">
         <v>256</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C16" s="30">
         <v>272</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13202,55 +13225,55 @@
         <v>57</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C17" s="30">
         <v>288</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C18" s="30">
         <v>304</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C19" s="30">
         <v>193</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C20" s="30">
         <v>209</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13258,55 +13281,55 @@
         <v>48</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C21" s="30">
         <v>225</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C22" s="30">
         <v>241</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C23" s="30">
         <v>257</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C24" s="30">
         <v>273</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13314,55 +13337,55 @@
         <v>57</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C25" s="30">
         <v>289</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C26" s="30">
         <v>305</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C27" s="30">
         <v>194</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C28" s="30">
         <v>210</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13370,55 +13393,55 @@
         <v>48</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C29" s="30">
         <v>226</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C30" s="30">
         <v>242</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C31" s="30">
         <v>258</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C32" s="30">
         <v>274</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13426,35 +13449,35 @@
         <v>57</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C33" s="30">
         <v>290</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C34" s="30">
         <v>306</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C35" s="30">
         <v>195</v>
@@ -13465,10 +13488,10 @@
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C36" s="30">
         <v>211</v>
@@ -13482,7 +13505,7 @@
         <v>48</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C37" s="30">
         <v>227</v>
@@ -13493,10 +13516,10 @@
     </row>
     <row r="38" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C38" s="30">
         <v>243</v>
@@ -13507,10 +13530,10 @@
     </row>
     <row r="39" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C39" s="30">
         <v>259</v>
@@ -13521,10 +13544,10 @@
     </row>
     <row r="40" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C40" s="30">
         <v>275</v>
@@ -13538,7 +13561,7 @@
         <v>57</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C41" s="30">
         <v>291</v>
@@ -13549,10 +13572,10 @@
     </row>
     <row r="42" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C42" s="30">
         <v>307</v>
@@ -13563,10 +13586,10 @@
     </row>
     <row r="43" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C43" s="30">
         <v>196</v>
@@ -13577,10 +13600,10 @@
     </row>
     <row r="44" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C44" s="30">
         <v>212</v>
@@ -13594,7 +13617,7 @@
         <v>48</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C45" s="30">
         <v>228</v>
@@ -13605,10 +13628,10 @@
     </row>
     <row r="46" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C46" s="30">
         <v>244</v>
@@ -13619,10 +13642,10 @@
     </row>
     <row r="47" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C47" s="30">
         <v>260</v>
@@ -13633,10 +13656,10 @@
     </row>
     <row r="48" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C48" s="30">
         <v>276</v>
@@ -13650,7 +13673,7 @@
         <v>57</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C49" s="30">
         <v>292</v>
@@ -13661,10 +13684,10 @@
     </row>
     <row r="50" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C50" s="30">
         <v>308</v>
@@ -14660,10 +14683,10 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Aggiornamento files test con ultime correzioni
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#CGMXX/CGM_XDENT_SOFTWARE_SRL/CGMXFSE/1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#CGMXX/CGM_XDENT_SOFTWARE_SRL/CGMXFSE/1/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/michele_bukovitz_cgm_com/Documents/Documentazione/FSE/ACCREDITAMENTO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="300" documentId="8_{45AC9EDC-DA0E-934D-A942-652691440C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7F7203D-4BDA-344D-9025-7FA6A1007CE7}"/>
+  <xr:revisionPtr revIDLastSave="333" documentId="8_{45AC9EDC-DA0E-934D-A942-652691440C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D204097D-4209-F049-81A5-920DC03016EA}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="500" windowWidth="34960" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="395">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1399,15 +1399,6 @@
     <t>e280bffe49e6d7d4</t>
   </si>
   <si>
-    <t>2024-04-18T18:43:07Z</t>
-  </si>
-  <si>
-    <t>03ed62e7733a6791</t>
-  </si>
-  <si>
-    <t>0.1.2.3.4.043066daf2109523a7490d4bfad4766da5719950a2b5f96d192fc0537e84f32a.c11d7205f8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2024-04-19T08:42:47Z</t>
   </si>
   <si>
@@ -1453,15 +1444,6 @@
     <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.002e6adad4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2024-04-19T10:18:50Z</t>
-  </si>
-  <si>
-    <t>ea341241cc4792a4</t>
-  </si>
-  <si>
-    <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.dc1b077efe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2024-04-19T10:23:08Z</t>
   </si>
   <si>
@@ -1505,12 +1487,6 @@
   </si>
   <si>
     <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.6552bbee88^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-04-19T10:40:34Z</t>
-  </si>
-  <si>
-    <t>e70939d610b27b02</t>
   </si>
   <si>
     <t>2024-04-19T10:58:55Z</t>
@@ -1575,15 +1551,6 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-04-23T09:14:26Z</t>
-  </si>
-  <si>
-    <t>a0643a4878275228</t>
-  </si>
-  <si>
-    <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.dab739dc51^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il sistema non contiene tutti i dati opzionali rappresentati in modo strutturato, in particolare la sezione conclusioni</t>
   </si>
   <si>
@@ -1648,6 +1615,42 @@
   </si>
   <si>
     <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.8cba2b19d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-06T14:54:59Z</t>
+  </si>
+  <si>
+    <t>c40af4c773868612</t>
+  </si>
+  <si>
+    <t>0.1.2.3.4.043066daf2109523a7490d4bfad4766da5719950a2b5f96d192fc0537e84f32a.223d195405^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4847a29914285c9a</t>
+  </si>
+  <si>
+    <t>2024-05-06T15:10:44Z</t>
+  </si>
+  <si>
+    <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.67cc11d250^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-06T15:13:41Z</t>
+  </si>
+  <si>
+    <t>f602599a93f25628</t>
+  </si>
+  <si>
+    <t>.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.0b71faf206^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-06T15:32:40Z</t>
+  </si>
+  <si>
+    <t>fd15add842421c3b</t>
+  </si>
+  <si>
+    <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.94bd59c5cc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2181,10 +2184,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4572,10 +4571,10 @@
   <dimension ref="A1:T700"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="79" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I69" sqref="I69"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4837,22 +4836,22 @@
         <v>48</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="F10" s="23">
-        <v>45405</v>
+        <v>45418</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>369</v>
+        <v>392</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>370</v>
+        <v>393</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>371</v>
+        <v>394</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>52</v>
@@ -4881,10 +4880,10 @@
         <v>48</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="F11" s="23">
         <v>45406</v>
@@ -4921,10 +4920,10 @@
         <v>48</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="F12" s="23">
         <v>45407</v>
@@ -4936,7 +4935,7 @@
         <v>81</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>
@@ -4961,10 +4960,10 @@
         <v>48</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="F13" s="23">
         <v>45408</v>
@@ -4976,7 +4975,7 @@
         <v>81</v>
       </c>
       <c r="K13" s="25" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -5010,10 +5009,10 @@
         <v>45401</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="I14" s="24" t="s">
         <v>51</v>
@@ -5118,10 +5117,10 @@
         <v>45401</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>51</v>
@@ -5175,7 +5174,7 @@
         <v>274</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>51</v>
@@ -5326,13 +5325,13 @@
         <v>45401</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>52</v>
@@ -5380,13 +5379,13 @@
         <v>45401</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>52</v>
@@ -5434,13 +5433,13 @@
         <v>45401</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>52</v>
@@ -5488,13 +5487,13 @@
         <v>45401</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>52</v>
@@ -5539,16 +5538,16 @@
         <v>76</v>
       </c>
       <c r="F24" s="23">
-        <v>45401</v>
+        <v>45418</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>331</v>
+        <v>389</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>332</v>
+        <v>390</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>333</v>
+        <v>391</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>52</v>
@@ -5596,13 +5595,13 @@
         <v>45401</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>52</v>
@@ -5688,13 +5687,13 @@
         <v>45401</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>52</v>
@@ -5780,13 +5779,13 @@
         <v>45401</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="J29" s="25" t="s">
         <v>52</v>
@@ -5834,13 +5833,13 @@
         <v>45401</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="H30" s="24" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="J30" s="25" t="s">
         <v>52</v>
@@ -6398,13 +6397,13 @@
         <v>45400</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>52</v>
@@ -7210,13 +7209,13 @@
         <v>45401</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="H62" s="24" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="J62" s="25" t="s">
         <v>52</v>
@@ -7292,10 +7291,10 @@
         <v>45401</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="H64" s="24" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="I64" s="24" t="s">
         <v>166</v>
@@ -7346,10 +7345,10 @@
         <v>45401</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H65" s="24" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="I65" s="24" t="s">
         <v>166</v>
@@ -7400,10 +7399,10 @@
         <v>45401</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H66" s="24" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="I66" s="24" t="s">
         <v>166</v>
@@ -7454,13 +7453,13 @@
         <v>45415</v>
       </c>
       <c r="G67" s="24" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="H67" s="24" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="I67" s="24" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="J67" s="25" t="s">
         <v>52</v>
@@ -7508,13 +7507,13 @@
         <v>45415</v>
       </c>
       <c r="G68" s="24" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="H68" s="24" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="J68" s="25" t="s">
         <v>52</v>
@@ -7562,13 +7561,13 @@
         <v>45415</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="H69" s="24" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="I69" s="24" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="J69" s="25" t="s">
         <v>52</v>
@@ -7616,7 +7615,7 @@
         <v>45400</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="H70" s="24" t="s">
         <v>299</v>
@@ -7698,7 +7697,7 @@
         <v>45400</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="H72" s="24" t="s">
         <v>301</v>
@@ -7752,7 +7751,7 @@
         <v>45400</v>
       </c>
       <c r="G73" s="24" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="H73" s="24" t="s">
         <v>302</v>
@@ -7806,7 +7805,7 @@
         <v>45400</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="H74" s="24" t="s">
         <v>303</v>
@@ -7860,7 +7859,7 @@
         <v>45400</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="H75" s="24" t="s">
         <v>305</v>
@@ -7914,7 +7913,7 @@
         <v>45400</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="H76" s="24" t="s">
         <v>307</v>
@@ -7968,7 +7967,7 @@
         <v>45400</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="H77" s="24" t="s">
         <v>309</v>
@@ -8022,10 +8021,10 @@
         <v>45401</v>
       </c>
       <c r="G78" s="24" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="H78" s="24" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="I78" s="24" t="s">
         <v>166</v>
@@ -8074,10 +8073,10 @@
         <v>45401</v>
       </c>
       <c r="G79" s="24" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="H79" s="24" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="I79" s="24" t="s">
         <v>166</v>
@@ -8215,16 +8214,16 @@
         <v>211</v>
       </c>
       <c r="F82" s="23">
-        <v>45401</v>
+        <v>45418</v>
       </c>
       <c r="G82" s="24" t="s">
-        <v>349</v>
+        <v>387</v>
       </c>
       <c r="H82" s="24" t="s">
-        <v>350</v>
+        <v>386</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>348</v>
+        <v>388</v>
       </c>
       <c r="J82" s="25" t="s">
         <v>52</v>
@@ -8259,16 +8258,16 @@
         <v>213</v>
       </c>
       <c r="F83" s="23">
-        <v>45400</v>
+        <v>45418</v>
       </c>
       <c r="G83" s="24" t="s">
-        <v>313</v>
+        <v>383</v>
       </c>
       <c r="H83" s="24" t="s">
-        <v>314</v>
+        <v>384</v>
       </c>
       <c r="I83" s="24" t="s">
-        <v>315</v>
+        <v>385</v>
       </c>
       <c r="J83" s="25" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Riesecuzione test 374 con recupero del risultato richiesto (VALIDAZIONE, nonn PUBBLICAZIONE).
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#CGMXX/CGM_XDENT_SOFTWARE_SRL/CGMXFSE/1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#CGMXX/CGM_XDENT_SOFTWARE_SRL/CGMXFSE/1/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/michele_bukovitz_cgm_com/Documents/Documentazione/FSE/ACCREDITAMENTO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="333" documentId="8_{45AC9EDC-DA0E-934D-A942-652691440C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D204097D-4209-F049-81A5-920DC03016EA}"/>
+  <xr:revisionPtr revIDLastSave="339" documentId="8_{45AC9EDC-DA0E-934D-A942-652691440C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAFD4DB4-C85A-8A4E-BA7D-C96741128D88}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="500" windowWidth="34960" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1617,12 +1617,6 @@
     <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.8cba2b19d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2024-05-06T14:54:59Z</t>
-  </si>
-  <si>
-    <t>c40af4c773868612</t>
-  </si>
-  <si>
     <t>0.1.2.3.4.043066daf2109523a7490d4bfad4766da5719950a2b5f96d192fc0537e84f32a.223d195405^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -1651,6 +1645,12 @@
   </si>
   <si>
     <t>0.1.2.3.4.620c9c332101a5bae955c66ae72268fbcd3972766179522c8deede6a249addb7.94bd59c5cc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-08T11:18:54Z</t>
+  </si>
+  <si>
+    <t>96684e2794d37039</t>
   </si>
 </sst>
 </file>
@@ -4571,10 +4571,10 @@
   <dimension ref="A1:T700"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="79" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4845,13 +4845,13 @@
         <v>45418</v>
       </c>
       <c r="G10" s="24" t="s">
+        <v>390</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="I10" s="24" t="s">
         <v>392</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>393</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>394</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>52</v>
@@ -5541,13 +5541,13 @@
         <v>45418</v>
       </c>
       <c r="G24" s="24" t="s">
+        <v>387</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>388</v>
+      </c>
+      <c r="I24" s="24" t="s">
         <v>389</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>390</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>391</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>52</v>
@@ -8217,13 +8217,13 @@
         <v>45418</v>
       </c>
       <c r="G82" s="24" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H82" s="24" t="s">
+        <v>384</v>
+      </c>
+      <c r="I82" s="24" t="s">
         <v>386</v>
-      </c>
-      <c r="I82" s="24" t="s">
-        <v>388</v>
       </c>
       <c r="J82" s="25" t="s">
         <v>52</v>
@@ -8258,16 +8258,16 @@
         <v>213</v>
       </c>
       <c r="F83" s="23">
-        <v>45418</v>
+        <v>45420</v>
       </c>
       <c r="G83" s="24" t="s">
+        <v>393</v>
+      </c>
+      <c r="H83" s="24" t="s">
+        <v>394</v>
+      </c>
+      <c r="I83" s="24" t="s">
         <v>383</v>
-      </c>
-      <c r="H83" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="I83" s="24" t="s">
-        <v>385</v>
       </c>
       <c r="J83" s="25" t="s">
         <v>52</v>

</xml_diff>